<commit_message>
Added some print statements
</commit_message>
<xml_diff>
--- a/test/mechanical/forecasts/ReportWeek3.xlsx
+++ b/test/mechanical/forecasts/ReportWeek3.xlsx
@@ -611,11 +611,11 @@
         <v>2</v>
       </c>
       <c r="B4" s="7">
-        <v>0.6867700743314346</v>
+        <v>0.6863962134059146</v>
       </c>
       <c r="C4" s="7"/>
       <c r="E4" s="7">
-        <v>0.6224239903212052</v>
+        <v>0.6215543264920883</v>
       </c>
       <c r="F4" s="7"/>
     </row>
@@ -624,11 +624,11 @@
         <v>3</v>
       </c>
       <c r="B5" s="6">
-        <v>44.00817410903709</v>
+        <v>43.98421712937564</v>
       </c>
       <c r="C5" s="6"/>
       <c r="E5" s="6">
-        <v>36.58243150768114</v>
+        <v>36.53131776856103</v>
       </c>
       <c r="F5" s="6"/>
     </row>
@@ -637,16 +637,16 @@
         <v>4</v>
       </c>
       <c r="B6" s="8">
-        <v>0.1830806</v>
+        <v>0.1829074</v>
       </c>
       <c r="C6" s="8">
-        <v>0.8169194</v>
+        <v>0.8170925999999999</v>
       </c>
       <c r="E6" s="8">
-        <v>0.8449136</v>
+        <v>0.8452689</v>
       </c>
       <c r="F6" s="8">
-        <v>0.1550864</v>
+        <v>0.1547311</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -654,16 +654,16 @@
         <v>5</v>
       </c>
       <c r="B7" s="9">
-        <v>20.7252904</v>
+        <v>20.7248214</v>
       </c>
       <c r="C7" s="9">
-        <v>30.3870406</v>
+        <v>30.3837742</v>
       </c>
       <c r="E7" s="9">
-        <v>30.3981708</v>
+        <v>30.3965046</v>
       </c>
       <c r="F7" s="9">
-        <v>21.5917508</v>
+        <v>21.5807964</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -739,7 +739,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="9">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C12" s="9">
         <v>26</v>
@@ -901,7 +901,7 @@
         <v>34</v>
       </c>
       <c r="F21" s="9">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:6">

</xml_diff>

<commit_message>
Moved N_SIMULATIONS from being hard-coded in  to set in the settings file
</commit_message>
<xml_diff>
--- a/test/mechanical/forecasts/ReportWeek3.xlsx
+++ b/test/mechanical/forecasts/ReportWeek3.xlsx
@@ -598,11 +598,11 @@
         <v>1</v>
       </c>
       <c r="B3" s="7">
-        <v>0.6407992391322337</v>
+        <v>0.6880700722480534</v>
       </c>
       <c r="C3" s="7"/>
       <c r="E3" s="7">
-        <v>0.5877413479644733</v>
+        <v>0.6397674343333133</v>
       </c>
       <c r="F3" s="7"/>
     </row>
@@ -611,11 +611,11 @@
         <v>2</v>
       </c>
       <c r="B4" s="7">
-        <v>0.6863962134059146</v>
+        <v>0.9973951713340502</v>
       </c>
       <c r="C4" s="7"/>
       <c r="E4" s="7">
-        <v>0.6215543264920883</v>
+        <v>0.01962905978144387</v>
       </c>
       <c r="F4" s="7"/>
     </row>
@@ -624,11 +624,11 @@
         <v>3</v>
       </c>
       <c r="B5" s="6">
-        <v>43.98421712937564</v>
+        <v>68.62777675996794</v>
       </c>
       <c r="C5" s="6"/>
       <c r="E5" s="6">
-        <v>36.53131776856103</v>
+        <v>1.255803321474957</v>
       </c>
       <c r="F5" s="6"/>
     </row>
@@ -637,16 +637,16 @@
         <v>4</v>
       </c>
       <c r="B6" s="8">
-        <v>0.1829074</v>
+        <v>0.469963</v>
       </c>
       <c r="C6" s="8">
-        <v>0.8170925999999999</v>
+        <v>0.530037</v>
       </c>
       <c r="E6" s="8">
-        <v>0.8452689</v>
+        <v>0.9981314999999999</v>
       </c>
       <c r="F6" s="8">
-        <v>0.1547311</v>
+        <v>0.0018685</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -654,16 +654,16 @@
         <v>5</v>
       </c>
       <c r="B7" s="9">
-        <v>20.7248214</v>
+        <v>26.505977</v>
       </c>
       <c r="C7" s="9">
-        <v>30.3837742</v>
+        <v>26.9429704</v>
       </c>
       <c r="E7" s="9">
-        <v>30.3965046</v>
+        <v>32.508251</v>
       </c>
       <c r="F7" s="9">
-        <v>21.5807964</v>
+        <v>16.0651154</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -671,16 +671,16 @@
         <v>6</v>
       </c>
       <c r="B8" s="9">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C8" s="9">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E8" s="9">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="F8" s="9">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -688,16 +688,16 @@
         <v>7</v>
       </c>
       <c r="B9" s="9">
+        <v>21</v>
+      </c>
+      <c r="C9" s="9">
+        <v>24</v>
+      </c>
+      <c r="E9" s="9">
+        <v>27</v>
+      </c>
+      <c r="F9" s="9">
         <v>10</v>
-      </c>
-      <c r="C9" s="9">
-        <v>20</v>
-      </c>
-      <c r="E9" s="9">
-        <v>23</v>
-      </c>
-      <c r="F9" s="9">
-        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -705,16 +705,16 @@
         <v>8</v>
       </c>
       <c r="B10" s="9">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="C10" s="9">
         <v>24</v>
       </c>
       <c r="E10" s="9">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="F10" s="9">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -722,16 +722,16 @@
         <v>9</v>
       </c>
       <c r="B11" s="9">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="C11" s="9">
         <v>25</v>
       </c>
       <c r="E11" s="9">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="F11" s="9">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -739,16 +739,16 @@
         <v>10</v>
       </c>
       <c r="B12" s="9">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="C12" s="9">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E12" s="9">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="F12" s="9">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -756,16 +756,16 @@
         <v>11</v>
       </c>
       <c r="B13" s="9">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C13" s="9">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E13" s="9">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F13" s="9">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -773,16 +773,16 @@
         <v>12</v>
       </c>
       <c r="B14" s="9">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C14" s="9">
         <v>27</v>
       </c>
       <c r="E14" s="9">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F14" s="9">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -790,16 +790,16 @@
         <v>13</v>
       </c>
       <c r="B15" s="9">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C15" s="9">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E15" s="9">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F15" s="9">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -807,16 +807,16 @@
         <v>14</v>
       </c>
       <c r="B16" s="9">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C16" s="9">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E16" s="9">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="F16" s="9">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -824,16 +824,16 @@
         <v>15</v>
       </c>
       <c r="B17" s="9">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C17" s="9">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E17" s="9">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F17" s="9">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -841,16 +841,16 @@
         <v>16</v>
       </c>
       <c r="B18" s="9">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C18" s="9">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E18" s="9">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F18" s="9">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -858,16 +858,16 @@
         <v>17</v>
       </c>
       <c r="B19" s="9">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C19" s="9">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E19" s="9">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F19" s="9">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -875,16 +875,16 @@
         <v>18</v>
       </c>
       <c r="B20" s="9">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="C20" s="9">
+        <v>28</v>
+      </c>
+      <c r="E20" s="9">
         <v>34</v>
       </c>
-      <c r="E20" s="9">
-        <v>33</v>
-      </c>
       <c r="F20" s="9">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -892,16 +892,16 @@
         <v>19</v>
       </c>
       <c r="B21" s="9">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="C21" s="9">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="E21" s="9">
         <v>34</v>
       </c>
       <c r="F21" s="9">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -909,16 +909,16 @@
         <v>20</v>
       </c>
       <c r="B22" s="9">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C22" s="9">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="E22" s="9">
         <v>34</v>
       </c>
       <c r="F22" s="9">
-        <v>27</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -926,16 +926,16 @@
         <v>21</v>
       </c>
       <c r="B23" s="9">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C23" s="9">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E23" s="9">
         <v>34</v>
       </c>
       <c r="F23" s="9">
-        <v>28</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -943,16 +943,16 @@
         <v>22</v>
       </c>
       <c r="B24" s="9">
+        <v>31</v>
+      </c>
+      <c r="C24" s="9">
         <v>30</v>
       </c>
-      <c r="C24" s="9">
-        <v>38</v>
-      </c>
       <c r="E24" s="9">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F24" s="9">
-        <v>29</v>
+        <v>20</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -963,13 +963,13 @@
         <v>31</v>
       </c>
       <c r="C25" s="9">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="E25" s="9">
         <v>38</v>
       </c>
       <c r="F25" s="9">
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -980,13 +980,13 @@
         <v>34</v>
       </c>
       <c r="C26" s="9">
+        <v>31</v>
+      </c>
+      <c r="E26" s="9">
         <v>41</v>
       </c>
-      <c r="E26" s="9">
-        <v>40</v>
-      </c>
       <c r="F26" s="9">
-        <v>31</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actually set n_simulations in the Game object
</commit_message>
<xml_diff>
--- a/test/mechanical/forecasts/ReportWeek3.xlsx
+++ b/test/mechanical/forecasts/ReportWeek3.xlsx
@@ -611,11 +611,11 @@
         <v>2</v>
       </c>
       <c r="B4" s="7">
-        <v>0.9973951713340502</v>
+        <v>0.9973667889636741</v>
       </c>
       <c r="C4" s="7"/>
       <c r="E4" s="7">
-        <v>0.01962905978144387</v>
+        <v>0.01956379902525768</v>
       </c>
       <c r="F4" s="7"/>
     </row>
@@ -624,11 +624,11 @@
         <v>3</v>
       </c>
       <c r="B5" s="6">
-        <v>68.62777675996794</v>
+        <v>68.62582385400442</v>
       </c>
       <c r="C5" s="6"/>
       <c r="E5" s="6">
-        <v>1.255803321474957</v>
+        <v>1.251628150820168</v>
       </c>
       <c r="F5" s="6"/>
     </row>
@@ -637,16 +637,16 @@
         <v>4</v>
       </c>
       <c r="B6" s="8">
-        <v>0.469963</v>
+        <v>0.4697999</v>
       </c>
       <c r="C6" s="8">
-        <v>0.530037</v>
+        <v>0.5302001</v>
       </c>
       <c r="E6" s="8">
-        <v>0.9981314999999999</v>
+        <v>0.9981387</v>
       </c>
       <c r="F6" s="8">
-        <v>0.0018685</v>
+        <v>0.0018613</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -654,16 +654,16 @@
         <v>5</v>
       </c>
       <c r="B7" s="9">
-        <v>26.505977</v>
+        <v>26.5061902</v>
       </c>
       <c r="C7" s="9">
-        <v>26.9429704</v>
+        <v>26.9440766</v>
       </c>
       <c r="E7" s="9">
-        <v>32.508251</v>
+        <v>32.50851</v>
       </c>
       <c r="F7" s="9">
-        <v>16.0651154</v>
+        <v>16.0670122</v>
       </c>
     </row>
     <row r="8" spans="1:6">

</xml_diff>

<commit_message>
Moved __weighted_variance(), __int2hex(), and __combine_colors() from load.py to util.py
</commit_message>
<xml_diff>
--- a/test/mechanical/forecasts/ReportWeek3.xlsx
+++ b/test/mechanical/forecasts/ReportWeek3.xlsx
@@ -611,11 +611,11 @@
         <v>2</v>
       </c>
       <c r="B4" s="7">
-        <v>0.9973667889636741</v>
+        <v>0.9973287529977295</v>
       </c>
       <c r="C4" s="7"/>
       <c r="E4" s="7">
-        <v>0.01956379902525768</v>
+        <v>0.01940319488623092</v>
       </c>
       <c r="F4" s="7"/>
     </row>
@@ -624,11 +624,11 @@
         <v>3</v>
       </c>
       <c r="B5" s="6">
-        <v>68.62582385400442</v>
+        <v>68.62320671302086</v>
       </c>
       <c r="C5" s="6"/>
       <c r="E5" s="6">
-        <v>1.251628150820168</v>
+        <v>1.241353221023322</v>
       </c>
       <c r="F5" s="6"/>
     </row>
@@ -637,16 +637,16 @@
         <v>4</v>
       </c>
       <c r="B6" s="8">
-        <v>0.4697999</v>
+        <v>0.4695827</v>
       </c>
       <c r="C6" s="8">
-        <v>0.5302001</v>
+        <v>0.5304173</v>
       </c>
       <c r="E6" s="8">
-        <v>0.9981387</v>
+        <v>0.9981564000000001</v>
       </c>
       <c r="F6" s="8">
-        <v>0.0018613</v>
+        <v>0.0018436</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -654,16 +654,16 @@
         <v>5</v>
       </c>
       <c r="B7" s="9">
-        <v>26.5061902</v>
+        <v>26.5027078</v>
       </c>
       <c r="C7" s="9">
-        <v>26.9440766</v>
+        <v>26.9435108</v>
       </c>
       <c r="E7" s="9">
-        <v>32.50851</v>
+        <v>32.5117888</v>
       </c>
       <c r="F7" s="9">
-        <v>16.0670122</v>
+        <v>16.068455</v>
       </c>
     </row>
     <row r="8" spans="1:6">

</xml_diff>

<commit_message>
Added most 2023 NFL Week 10 results and restructured some files (including creation of calculate module)
</commit_message>
<xml_diff>
--- a/test/mechanical/forecasts/ReportWeek3.xlsx
+++ b/test/mechanical/forecasts/ReportWeek3.xlsx
@@ -611,11 +611,11 @@
         <v>2</v>
       </c>
       <c r="B4" s="7">
-        <v>0.9973287529977295</v>
+        <v>0.9973508863433136</v>
       </c>
       <c r="C4" s="7"/>
       <c r="E4" s="7">
-        <v>0.01940319488623092</v>
+        <v>0.01918230390331595</v>
       </c>
       <c r="F4" s="7"/>
     </row>
@@ -624,11 +624,11 @@
         <v>3</v>
       </c>
       <c r="B5" s="6">
-        <v>68.62320671302086</v>
+        <v>68.62472964229038</v>
       </c>
       <c r="C5" s="6"/>
       <c r="E5" s="6">
-        <v>1.241353221023322</v>
+        <v>1.227221335282634</v>
       </c>
       <c r="F5" s="6"/>
     </row>
@@ -637,16 +637,16 @@
         <v>4</v>
       </c>
       <c r="B6" s="8">
-        <v>0.4695827</v>
+        <v>0.4697089</v>
       </c>
       <c r="C6" s="8">
-        <v>0.5304173</v>
+        <v>0.5302911</v>
       </c>
       <c r="E6" s="8">
-        <v>0.9981564000000001</v>
+        <v>0.9981807</v>
       </c>
       <c r="F6" s="8">
-        <v>0.0018436</v>
+        <v>0.0018193</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -654,16 +654,16 @@
         <v>5</v>
       </c>
       <c r="B7" s="9">
-        <v>26.5027078</v>
+        <v>26.5056628</v>
       </c>
       <c r="C7" s="9">
-        <v>26.9435108</v>
+        <v>26.944527</v>
       </c>
       <c r="E7" s="9">
-        <v>32.5117888</v>
+        <v>32.5121498</v>
       </c>
       <c r="F7" s="9">
-        <v>16.068455</v>
+        <v>16.0645064</v>
       </c>
     </row>
     <row r="8" spans="1:6">

</xml_diff>

<commit_message>
Added comments and cleaned up code
</commit_message>
<xml_diff>
--- a/test/mechanical/forecasts/ReportWeek3.xlsx
+++ b/test/mechanical/forecasts/ReportWeek3.xlsx
@@ -611,11 +611,11 @@
         <v>2</v>
       </c>
       <c r="B4" s="7">
-        <v>0.9973508863433136</v>
+        <v>0.9973886071615455</v>
       </c>
       <c r="C4" s="7"/>
       <c r="E4" s="7">
-        <v>0.01918230390331595</v>
+        <v>0.01952933962840083</v>
       </c>
       <c r="F4" s="7"/>
     </row>
@@ -624,11 +624,11 @@
         <v>3</v>
       </c>
       <c r="B5" s="6">
-        <v>68.62472964229038</v>
+        <v>68.62732509890299</v>
       </c>
       <c r="C5" s="6"/>
       <c r="E5" s="6">
-        <v>1.227221335282634</v>
+        <v>1.24942355082859</v>
       </c>
       <c r="F5" s="6"/>
     </row>
@@ -637,16 +637,16 @@
         <v>4</v>
       </c>
       <c r="B6" s="8">
-        <v>0.4697089</v>
+        <v>0.4699252</v>
       </c>
       <c r="C6" s="8">
-        <v>0.5302911</v>
+        <v>0.5300748</v>
       </c>
       <c r="E6" s="8">
-        <v>0.9981807</v>
+        <v>0.9981425</v>
       </c>
       <c r="F6" s="8">
-        <v>0.0018193</v>
+        <v>0.0018575</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -654,16 +654,16 @@
         <v>5</v>
       </c>
       <c r="B7" s="9">
-        <v>26.5056628</v>
+        <v>26.5073196</v>
       </c>
       <c r="C7" s="9">
-        <v>26.944527</v>
+        <v>26.943518</v>
       </c>
       <c r="E7" s="9">
-        <v>32.5121498</v>
+        <v>32.5092004</v>
       </c>
       <c r="F7" s="9">
-        <v>16.0645064</v>
+        <v>16.0649512</v>
       </c>
     </row>
     <row r="8" spans="1:6">

</xml_diff>